<commit_message>
upated excel and script
</commit_message>
<xml_diff>
--- a/Swapnotory/DataBase And Application/adm_code_elements.xlsx
+++ b/Swapnotory/DataBase And Application/adm_code_elements.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="137">
   <si>
     <t>ELEMENT_ID</t>
   </si>
@@ -59,18 +59,45 @@
     <t>UPDATED_AT</t>
   </si>
   <si>
+    <t>ACE-02</t>
+  </si>
+  <si>
+    <t>Director of Administration</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>ACE-07</t>
+  </si>
+  <si>
+    <t>Advisory Member</t>
+  </si>
+  <si>
+    <t>Brac Bank</t>
+  </si>
+  <si>
+    <t>City Bank</t>
+  </si>
+  <si>
+    <t>Break Even Point</t>
+  </si>
+  <si>
+    <t>IFIC Bank</t>
+  </si>
+  <si>
+    <t>Postponed</t>
+  </si>
+  <si>
+    <t>Successfully Complete</t>
+  </si>
+  <si>
     <t>ACE-01</t>
   </si>
   <si>
     <t>A+</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>ACE-02</t>
-  </si>
-  <si>
     <t>AB+</t>
   </si>
   <si>
@@ -86,163 +113,313 @@
     <t>Staffs</t>
   </si>
   <si>
+    <t>Users</t>
+  </si>
+  <si>
     <t>ACE-04</t>
   </si>
   <si>
+    <t>O+</t>
+  </si>
+  <si>
+    <t>ACE-HR-H</t>
+  </si>
+  <si>
+    <t>ACE-USER</t>
+  </si>
+  <si>
+    <t>HR Officials</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>ACE-HR-CU</t>
+  </si>
+  <si>
+    <t>ACE-USER-CU</t>
+  </si>
+  <si>
+    <t>Customers</t>
+  </si>
+  <si>
+    <t>ACE-HR</t>
+  </si>
+  <si>
+    <t>ACE-CLIENTS</t>
+  </si>
+  <si>
+    <t>Clients</t>
+  </si>
+  <si>
+    <t>ACE-SYSTEM</t>
+  </si>
+  <si>
+    <t>System Admin</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Operation And Communication</t>
+  </si>
+  <si>
+    <t>Bank</t>
+  </si>
+  <si>
+    <t>Bkash</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>ACE-3</t>
+  </si>
+  <si>
+    <t>Divorced</t>
+  </si>
+  <si>
+    <t>ACE-JAN</t>
+  </si>
+  <si>
+    <t>JANUARY</t>
+  </si>
+  <si>
+    <t>ACE-FEB</t>
+  </si>
+  <si>
+    <t>FEBRUARY</t>
+  </si>
+  <si>
+    <t>ACE-MAR</t>
+  </si>
+  <si>
+    <t>MARCH</t>
+  </si>
+  <si>
+    <t>ACE-APR</t>
+  </si>
+  <si>
+    <t>APRIL</t>
+  </si>
+  <si>
+    <t>ACE-MAY</t>
+  </si>
+  <si>
+    <t>MAY</t>
+  </si>
+  <si>
+    <t>ACE-JUNE</t>
+  </si>
+  <si>
+    <t>JUNE</t>
+  </si>
+  <si>
+    <t>ACE-JULY</t>
+  </si>
+  <si>
+    <t>JULY</t>
+  </si>
+  <si>
+    <t>ACE-AUG</t>
+  </si>
+  <si>
+    <t>AUGUST</t>
+  </si>
+  <si>
+    <t>ACE-SEP</t>
+  </si>
+  <si>
+    <t>SEPTEMBER</t>
+  </si>
+  <si>
+    <t>ACE-OCT</t>
+  </si>
+  <si>
+    <t>OCTOBER</t>
+  </si>
+  <si>
+    <t>ACE-NOV</t>
+  </si>
+  <si>
+    <t>NOVEMBER</t>
+  </si>
+  <si>
+    <t>ACE-DEC</t>
+  </si>
+  <si>
+    <t>DECEMBER</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Islam</t>
+  </si>
+  <si>
+    <t>Hindu</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>Chirstian</t>
+  </si>
+  <si>
+    <t>Buddhist</t>
+  </si>
+  <si>
+    <t>AB Bank PLC</t>
+  </si>
+  <si>
+    <t>Bank Asia Limited</t>
+  </si>
+  <si>
+    <t>Director of Marketing</t>
+  </si>
+  <si>
+    <t>ACE-05</t>
+  </si>
+  <si>
+    <t>Project Coordinator</t>
+  </si>
+  <si>
+    <t>ACE-06</t>
+  </si>
+  <si>
+    <t>Presidium Member</t>
+  </si>
+  <si>
+    <t>Rocket</t>
+  </si>
+  <si>
+    <t>Travel Expenses</t>
+  </si>
+  <si>
+    <t>Travel Expenses:</t>
+  </si>
+  <si>
+    <t>Meals and Entertainment</t>
+  </si>
+  <si>
+    <t>Meals and Entertainment:</t>
+  </si>
+  <si>
+    <t>Office Supplies</t>
+  </si>
+  <si>
+    <t>Utilities</t>
+  </si>
+  <si>
+    <t>Rent or Mortgage</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>Employee Salaries</t>
+  </si>
+  <si>
+    <t>Taxes</t>
+  </si>
+  <si>
+    <t>Maintenance and Repairs</t>
+  </si>
+  <si>
+    <t>Marketing and Advertising</t>
+  </si>
+  <si>
+    <t>Training and Education</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>Al-Arafah Islami Bank PLC</t>
+  </si>
+  <si>
+    <t>EXIM Bank PLC</t>
+  </si>
+  <si>
+    <t>First Security Islami Bank PLC</t>
+  </si>
+  <si>
+    <t>Global Islami Bank PLC</t>
+  </si>
+  <si>
+    <t>Islami Bank Bangladesh PLC</t>
+  </si>
+  <si>
+    <t>Shahjalal Islami Bank PLC</t>
+  </si>
+  <si>
+    <t>ACE-08</t>
+  </si>
+  <si>
+    <t>N/D</t>
+  </si>
+  <si>
+    <t>Director of Finance</t>
+  </si>
+  <si>
+    <t>Premier Bank</t>
+  </si>
+  <si>
+    <t>Dutch Bangla Bank</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Nagad</t>
+  </si>
+  <si>
     <t>A-</t>
   </si>
   <si>
-    <t>ACE-HR-H</t>
-  </si>
-  <si>
-    <t>ACE-USER</t>
-  </si>
-  <si>
-    <t>HR Officials</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>ACE-HR-CU</t>
-  </si>
-  <si>
-    <t>ACE-USER-CU</t>
-  </si>
-  <si>
-    <t>Customers</t>
-  </si>
-  <si>
-    <t>ACE-HR</t>
-  </si>
-  <si>
-    <t>ACE-CLIENTS</t>
-  </si>
-  <si>
-    <t>Clients</t>
-  </si>
-  <si>
-    <t>ACE-SYSTEM</t>
-  </si>
-  <si>
-    <t>System Admin</t>
-  </si>
-  <si>
-    <t>Cash</t>
-  </si>
-  <si>
-    <t>Cheque</t>
-  </si>
-  <si>
-    <t>Bank</t>
-  </si>
-  <si>
-    <t>Bkash</t>
-  </si>
-  <si>
-    <t>Single</t>
-  </si>
-  <si>
-    <t>Married</t>
-  </si>
-  <si>
-    <t>ACE-3</t>
-  </si>
-  <si>
-    <t>Divorced</t>
-  </si>
-  <si>
-    <t>ACE-JAN</t>
-  </si>
-  <si>
-    <t>JANUARY</t>
-  </si>
-  <si>
-    <t>ACE-FEB</t>
-  </si>
-  <si>
-    <t>FEBRUARY</t>
-  </si>
-  <si>
-    <t>ACE-MAR</t>
-  </si>
-  <si>
-    <t>MARCH</t>
-  </si>
-  <si>
-    <t>ACE-APR</t>
-  </si>
-  <si>
-    <t>APRIL</t>
-  </si>
-  <si>
-    <t>ACE-MAY</t>
-  </si>
-  <si>
-    <t>MAY</t>
-  </si>
-  <si>
-    <t>ACE-JUNE</t>
-  </si>
-  <si>
-    <t>JUNE</t>
-  </si>
-  <si>
-    <t>ACE-JULY</t>
-  </si>
-  <si>
-    <t>JULY</t>
-  </si>
-  <si>
-    <t>ACE-AUG</t>
-  </si>
-  <si>
-    <t>AUGUST</t>
-  </si>
-  <si>
-    <t>ACE-SEP</t>
-  </si>
-  <si>
-    <t>SEPTEMBER</t>
-  </si>
-  <si>
-    <t>ACE-OCT</t>
-  </si>
-  <si>
-    <t>OCTOBER</t>
-  </si>
-  <si>
-    <t>ACE-NOV</t>
-  </si>
-  <si>
-    <t>NOVEMBER</t>
-  </si>
-  <si>
-    <t>ACE-DEC</t>
-  </si>
-  <si>
-    <t>DECEMBER</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>Islam</t>
-  </si>
-  <si>
-    <t>Hindu</t>
-  </si>
-  <si>
-    <t>Christian</t>
-  </si>
-  <si>
-    <t>Chirstian</t>
-  </si>
-  <si>
-    <t>Buddhist</t>
+    <t>Eastern Bank</t>
+  </si>
+  <si>
+    <t>Bank Asia</t>
+  </si>
+  <si>
+    <t>Prime Bank</t>
+  </si>
+  <si>
+    <t>Upcoming</t>
+  </si>
+  <si>
+    <t>Bangladesh Commerce Bank Limit</t>
+  </si>
+  <si>
+    <t>Bangladesh Commerce Bank Limited</t>
+  </si>
+  <si>
+    <t>AB-</t>
+  </si>
+  <si>
+    <t>B-</t>
+  </si>
+  <si>
+    <t>O-</t>
+  </si>
+  <si>
+    <t>Finance Member</t>
+  </si>
+  <si>
+    <t>Monthly Statement</t>
   </si>
 </sst>
 </file>
@@ -342,8 +519,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" displayName="sheet1" ref="A1:P36" totalsRowShown="0" headerRowCount="1">
-  <autoFilter ref="A1:P36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" displayName="sheet1" ref="A1:P90" totalsRowShown="0" headerRowCount="1">
+  <autoFilter ref="A1:P90"/>
   <tableColumns count="16">
     <tableColumn id="1" name="ELEMENT_ID"/>
     <tableColumn id="2" name="CODE_ID"/>
@@ -377,12 +554,12 @@
   <cols>
     <col min="1" max="1" width="17.18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.64" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.55" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.82" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.82" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.73" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.55" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.55" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.45" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.91" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.18" bestFit="1" customWidth="1"/>
@@ -445,10 +622,10 @@
     </row>
     <row r="2" customHeight="1" ht="20">
       <c r="A2" s="5" t="n">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="B2" s="5" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>16</v>
@@ -461,9 +638,7 @@
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="H2" s="6"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
@@ -474,17 +649,19 @@
         <v>1000</v>
       </c>
       <c r="N2" s="7" t="n">
-        <v>45183</v>
+        <v>45319</v>
       </c>
       <c r="O2" s="5"/>
-      <c r="P2" s="7"/>
+      <c r="P2" s="7" t="n">
+        <v>45321.4724884259</v>
+      </c>
     </row>
     <row r="3" customHeight="1" ht="20">
       <c r="A3" s="5" t="n">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>19</v>
@@ -497,9 +674,7 @@
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="H3" s="6"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -510,17 +685,17 @@
         <v>1000</v>
       </c>
       <c r="N3" s="7" t="n">
-        <v>45183</v>
+        <v>45319</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="7"/>
     </row>
     <row r="4" customHeight="1" ht="20">
       <c r="A4" s="5" t="n">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>21</v>
@@ -529,12 +704,12 @@
         <v>21</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -546,31 +721,31 @@
         <v>1000</v>
       </c>
       <c r="N4" s="7" t="n">
-        <v>45183</v>
+        <v>45321</v>
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="7"/>
     </row>
     <row r="5" customHeight="1" ht="20">
       <c r="A5" s="5" t="n">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -582,17 +757,17 @@
         <v>1000</v>
       </c>
       <c r="N5" s="7" t="n">
-        <v>45182</v>
+        <v>45321</v>
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="7"/>
     </row>
     <row r="6" customHeight="1" ht="20">
       <c r="A6" s="5" t="n">
-        <v>38</v>
+        <v>119</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>23</v>
@@ -601,12 +776,12 @@
         <v>23</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
@@ -618,31 +793,33 @@
         <v>1000</v>
       </c>
       <c r="N6" s="7" t="n">
-        <v>45182</v>
+        <v>45323</v>
       </c>
       <c r="O6" s="5"/>
-      <c r="P6" s="7"/>
+      <c r="P6" s="7" t="n">
+        <v>45323.1647685185</v>
+      </c>
     </row>
     <row r="7" customHeight="1" ht="20">
       <c r="A7" s="5" t="n">
-        <v>67</v>
+        <v>124</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -654,145 +831,141 @@
         <v>1000</v>
       </c>
       <c r="N7" s="7" t="n">
-        <v>45227</v>
+        <v>45323</v>
       </c>
       <c r="O7" s="5"/>
       <c r="P7" s="7"/>
     </row>
     <row r="8" customHeight="1" ht="20">
       <c r="A8" s="5" t="n">
-        <v>33</v>
+        <v>125</v>
       </c>
       <c r="B8" s="5" t="n">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="M8" s="5" t="n">
         <v>1000</v>
       </c>
       <c r="N8" s="7" t="n">
-        <v>45182</v>
+        <v>45323</v>
       </c>
       <c r="O8" s="5"/>
-      <c r="P8" s="7" t="n">
-        <v>45229.357337963</v>
-      </c>
+      <c r="P8" s="7"/>
     </row>
     <row r="9" customHeight="1" ht="20">
       <c r="A9" s="5" t="n">
-        <v>34</v>
+        <v>127</v>
       </c>
       <c r="B9" s="5" t="n">
+        <v>47</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="D9" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="M9" s="5" t="n">
         <v>1000</v>
       </c>
       <c r="N9" s="7" t="n">
-        <v>45182</v>
+        <v>45323</v>
       </c>
       <c r="O9" s="5"/>
       <c r="P9" s="7" t="n">
-        <v>45229.357337963</v>
+        <v>45323.2394212963</v>
       </c>
     </row>
     <row r="10" customHeight="1" ht="20">
       <c r="A10" s="5" t="n">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="B10" s="5" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="M10" s="5" t="n">
         <v>1000</v>
       </c>
       <c r="N10" s="7" t="n">
-        <v>45182</v>
+        <v>45183</v>
       </c>
       <c r="O10" s="5"/>
-      <c r="P10" s="7" t="n">
-        <v>45229.357337963</v>
-      </c>
+      <c r="P10" s="7"/>
     </row>
     <row r="11" customHeight="1" ht="20">
       <c r="A11" s="5" t="n">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="B11" s="5" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -804,31 +977,31 @@
         <v>1000</v>
       </c>
       <c r="N11" s="7" t="n">
-        <v>45182</v>
+        <v>45183</v>
       </c>
       <c r="O11" s="5"/>
       <c r="P11" s="7"/>
     </row>
     <row r="12" customHeight="1" ht="20">
       <c r="A12" s="5" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="5" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
@@ -840,107 +1013,105 @@
         <v>1000</v>
       </c>
       <c r="N12" s="7" t="n">
-        <v>45184</v>
+        <v>45183</v>
       </c>
       <c r="O12" s="5"/>
       <c r="P12" s="7"/>
     </row>
     <row r="13" customHeight="1" ht="20">
       <c r="A13" s="5" t="n">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B13" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>40</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="M13" s="5" t="n">
         <v>1000</v>
       </c>
       <c r="N13" s="7" t="n">
-        <v>45184</v>
+        <v>45182</v>
       </c>
       <c r="O13" s="5"/>
-      <c r="P13" s="7" t="n">
-        <v>45192.5583449074</v>
-      </c>
+      <c r="P13" s="7"/>
     </row>
     <row r="14" customHeight="1" ht="20">
       <c r="A14" s="5" t="n">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B14" s="5" t="n">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="M14" s="5" t="n">
         <v>1000</v>
       </c>
       <c r="N14" s="7" t="n">
-        <v>45184</v>
+        <v>45182</v>
       </c>
       <c r="O14" s="5"/>
       <c r="P14" s="7" t="n">
-        <v>45192.5583449074</v>
+        <v>45313.6711805556</v>
       </c>
     </row>
     <row r="15" customHeight="1" ht="20">
       <c r="A15" s="5" t="n">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="B15" s="5" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -952,92 +1123,98 @@
         <v>1000</v>
       </c>
       <c r="N15" s="7" t="n">
-        <v>45184</v>
+        <v>45227</v>
       </c>
       <c r="O15" s="5"/>
-      <c r="P15" s="7"/>
+      <c r="P15" s="7" t="n">
+        <v>45315.7279166667</v>
+      </c>
     </row>
     <row r="16" customHeight="1" ht="20">
       <c r="A16" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="B16" s="5" t="n">
+        <v>26</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="B16" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="6" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="M16" s="5" t="n">
         <v>1000</v>
       </c>
       <c r="N16" s="7" t="n">
-        <v>45183</v>
+        <v>45182</v>
       </c>
       <c r="O16" s="5"/>
-      <c r="P16" s="7"/>
+      <c r="P16" s="7" t="n">
+        <v>45229.357337963</v>
+      </c>
     </row>
     <row r="17" customHeight="1" ht="20">
       <c r="A17" s="5" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B17" s="5" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="6" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="M17" s="5" t="n">
         <v>1000</v>
       </c>
       <c r="N17" s="7" t="n">
-        <v>45183</v>
+        <v>45182</v>
       </c>
       <c r="O17" s="5"/>
-      <c r="P17" s="7"/>
+      <c r="P17" s="7" t="n">
+        <v>45229.357337963</v>
+      </c>
     </row>
     <row r="18" customHeight="1" ht="20">
       <c r="A18" s="5" t="n">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B18" s="5" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>45</v>
@@ -1054,23 +1231,25 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="6" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="M18" s="5" t="n">
         <v>1000</v>
       </c>
       <c r="N18" s="7" t="n">
-        <v>45183</v>
+        <v>45182</v>
       </c>
       <c r="O18" s="5"/>
-      <c r="P18" s="7"/>
+      <c r="P18" s="7" t="n">
+        <v>45229.357337963</v>
+      </c>
     </row>
     <row r="19" customHeight="1" ht="20">
       <c r="A19" s="5" t="n">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="B19" s="5" t="n">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>47</v>
@@ -1096,31 +1275,31 @@
         <v>1000</v>
       </c>
       <c r="N19" s="7" t="n">
-        <v>45192</v>
+        <v>45182</v>
       </c>
       <c r="O19" s="5"/>
       <c r="P19" s="7"/>
     </row>
     <row r="20" customHeight="1" ht="20">
       <c r="A20" s="5" t="n">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B20" s="5" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -1132,32 +1311,30 @@
         <v>1000</v>
       </c>
       <c r="N20" s="7" t="n">
-        <v>45192</v>
+        <v>45184</v>
       </c>
       <c r="O20" s="5"/>
       <c r="P20" s="7"/>
     </row>
     <row r="21" customHeight="1" ht="20">
       <c r="A21" s="5" t="n">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="B21" s="5" t="n">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="6" t="s">
-        <v>52</v>
-      </c>
+      <c r="H21" s="6"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -1168,31 +1345,31 @@
         <v>1000</v>
       </c>
       <c r="N21" s="7" t="n">
-        <v>45192</v>
+        <v>45319</v>
       </c>
       <c r="O21" s="5"/>
       <c r="P21" s="7"/>
     </row>
     <row r="22" customHeight="1" ht="20">
       <c r="A22" s="5" t="n">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B22" s="5" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
@@ -1204,31 +1381,33 @@
         <v>1000</v>
       </c>
       <c r="N22" s="7" t="n">
-        <v>45192</v>
+        <v>45184</v>
       </c>
       <c r="O22" s="5"/>
-      <c r="P22" s="7"/>
+      <c r="P22" s="7" t="n">
+        <v>45313.6857060185</v>
+      </c>
     </row>
     <row r="23" customHeight="1" ht="20">
       <c r="A23" s="5" t="n">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B23" s="5" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
@@ -1240,31 +1419,31 @@
         <v>1000</v>
       </c>
       <c r="N23" s="7" t="n">
-        <v>45192</v>
+        <v>45184</v>
       </c>
       <c r="O23" s="5"/>
       <c r="P23" s="7"/>
     </row>
     <row r="24" customHeight="1" ht="20">
       <c r="A24" s="5" t="n">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="B24" s="5" t="n">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
@@ -1276,31 +1455,31 @@
         <v>1000</v>
       </c>
       <c r="N24" s="7" t="n">
-        <v>45192</v>
+        <v>45183</v>
       </c>
       <c r="O24" s="5"/>
       <c r="P24" s="7"/>
     </row>
     <row r="25" customHeight="1" ht="20">
       <c r="A25" s="5" t="n">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="B25" s="5" t="n">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
@@ -1312,31 +1491,31 @@
         <v>1000</v>
       </c>
       <c r="N25" s="7" t="n">
-        <v>45192</v>
+        <v>45183</v>
       </c>
       <c r="O25" s="5"/>
       <c r="P25" s="7"/>
     </row>
     <row r="26" customHeight="1" ht="20">
       <c r="A26" s="5" t="n">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="B26" s="5" t="n">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
@@ -1348,31 +1527,31 @@
         <v>1000</v>
       </c>
       <c r="N26" s="7" t="n">
-        <v>45192</v>
+        <v>45183</v>
       </c>
       <c r="O26" s="5"/>
       <c r="P26" s="7"/>
     </row>
     <row r="27" customHeight="1" ht="20">
       <c r="A27" s="5" t="n">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B27" s="5" t="n">
         <v>34</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
@@ -1391,24 +1570,24 @@
     </row>
     <row r="28" customHeight="1" ht="20">
       <c r="A28" s="5" t="n">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B28" s="5" t="n">
         <v>34</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
@@ -1427,24 +1606,24 @@
     </row>
     <row r="29" customHeight="1" ht="20">
       <c r="A29" s="5" t="n">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B29" s="5" t="n">
         <v>34</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
@@ -1463,24 +1642,24 @@
     </row>
     <row r="30" customHeight="1" ht="20">
       <c r="A30" s="5" t="n">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B30" s="5" t="n">
         <v>34</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
@@ -1499,24 +1678,24 @@
     </row>
     <row r="31" customHeight="1" ht="20">
       <c r="A31" s="5" t="n">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B31" s="5" t="n">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
@@ -1528,31 +1707,31 @@
         <v>1000</v>
       </c>
       <c r="N31" s="7" t="n">
-        <v>45183</v>
+        <v>45192</v>
       </c>
       <c r="O31" s="5"/>
       <c r="P31" s="7"/>
     </row>
     <row r="32" customHeight="1" ht="20">
       <c r="A32" s="5" t="n">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B32" s="5" t="n">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
@@ -1564,31 +1743,31 @@
         <v>1000</v>
       </c>
       <c r="N32" s="7" t="n">
-        <v>45183</v>
+        <v>45192</v>
       </c>
       <c r="O32" s="5"/>
       <c r="P32" s="7"/>
     </row>
     <row r="33" customHeight="1" ht="20">
       <c r="A33" s="5" t="n">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B33" s="5" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
@@ -1600,31 +1779,31 @@
         <v>1000</v>
       </c>
       <c r="N33" s="7" t="n">
-        <v>45183</v>
+        <v>45192</v>
       </c>
       <c r="O33" s="5"/>
       <c r="P33" s="7"/>
     </row>
     <row r="34" customHeight="1" ht="20">
       <c r="A34" s="5" t="n">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B34" s="5" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
@@ -1636,31 +1815,31 @@
         <v>1000</v>
       </c>
       <c r="N34" s="7" t="n">
-        <v>45183</v>
+        <v>45192</v>
       </c>
       <c r="O34" s="5"/>
       <c r="P34" s="7"/>
     </row>
     <row r="35" customHeight="1" ht="20">
       <c r="A35" s="5" t="n">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="B35" s="5" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
       <c r="H35" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
@@ -1672,31 +1851,31 @@
         <v>1000</v>
       </c>
       <c r="N35" s="7" t="n">
-        <v>45183</v>
+        <v>45192</v>
       </c>
       <c r="O35" s="5"/>
       <c r="P35" s="7"/>
     </row>
     <row r="36" customHeight="1" ht="20">
       <c r="A36" s="5" t="n">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="B36" s="5" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
@@ -1708,10 +1887,1956 @@
         <v>1000</v>
       </c>
       <c r="N36" s="7" t="n">
-        <v>45183</v>
+        <v>45192</v>
       </c>
       <c r="O36" s="5"/>
       <c r="P36" s="7"/>
+    </row>
+    <row r="37" customHeight="1" ht="20">
+      <c r="A37" s="5" t="n">
+        <v>65</v>
+      </c>
+      <c r="B37" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M37" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N37" s="7" t="n">
+        <v>45192</v>
+      </c>
+      <c r="O37" s="5"/>
+      <c r="P37" s="7"/>
+    </row>
+    <row r="38" customHeight="1" ht="20">
+      <c r="A38" s="5" t="n">
+        <v>66</v>
+      </c>
+      <c r="B38" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M38" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N38" s="7" t="n">
+        <v>45192</v>
+      </c>
+      <c r="O38" s="5"/>
+      <c r="P38" s="7"/>
+    </row>
+    <row r="39" customHeight="1" ht="20">
+      <c r="A39" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="B39" s="5" t="n">
+        <v>29</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M39" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N39" s="7" t="n">
+        <v>45183</v>
+      </c>
+      <c r="O39" s="5"/>
+      <c r="P39" s="7"/>
+    </row>
+    <row r="40" customHeight="1" ht="20">
+      <c r="A40" s="5" t="n">
+        <v>43</v>
+      </c>
+      <c r="B40" s="5" t="n">
+        <v>29</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M40" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N40" s="7" t="n">
+        <v>45183</v>
+      </c>
+      <c r="O40" s="5"/>
+      <c r="P40" s="7"/>
+    </row>
+    <row r="41" customHeight="1" ht="20">
+      <c r="A41" s="5" t="n">
+        <v>44</v>
+      </c>
+      <c r="B41" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M41" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N41" s="7" t="n">
+        <v>45183</v>
+      </c>
+      <c r="O41" s="5"/>
+      <c r="P41" s="7"/>
+    </row>
+    <row r="42" customHeight="1" ht="20">
+      <c r="A42" s="5" t="n">
+        <v>45</v>
+      </c>
+      <c r="B42" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M42" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N42" s="7" t="n">
+        <v>45183</v>
+      </c>
+      <c r="O42" s="5"/>
+      <c r="P42" s="7"/>
+    </row>
+    <row r="43" customHeight="1" ht="20">
+      <c r="A43" s="5" t="n">
+        <v>46</v>
+      </c>
+      <c r="B43" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M43" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N43" s="7" t="n">
+        <v>45183</v>
+      </c>
+      <c r="O43" s="5"/>
+      <c r="P43" s="7"/>
+    </row>
+    <row r="44" customHeight="1" ht="20">
+      <c r="A44" s="5" t="n">
+        <v>47</v>
+      </c>
+      <c r="B44" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M44" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N44" s="7" t="n">
+        <v>45183</v>
+      </c>
+      <c r="O44" s="5"/>
+      <c r="P44" s="7"/>
+    </row>
+    <row r="45" customHeight="1" ht="20">
+      <c r="A45" s="5" t="n">
+        <v>70</v>
+      </c>
+      <c r="B45" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M45" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N45" s="7" t="n">
+        <v>45313</v>
+      </c>
+      <c r="O45" s="5"/>
+      <c r="P45" s="7"/>
+    </row>
+    <row r="46" customHeight="1" ht="20">
+      <c r="A46" s="5" t="n">
+        <v>72</v>
+      </c>
+      <c r="B46" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M46" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N46" s="7" t="n">
+        <v>45313</v>
+      </c>
+      <c r="O46" s="5"/>
+      <c r="P46" s="7"/>
+    </row>
+    <row r="47" customHeight="1" ht="20">
+      <c r="A47" s="5" t="n">
+        <v>86</v>
+      </c>
+      <c r="B47" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M47" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N47" s="7" t="n">
+        <v>45319</v>
+      </c>
+      <c r="O47" s="5"/>
+      <c r="P47" s="7" t="n">
+        <v>45321.4723032407</v>
+      </c>
+    </row>
+    <row r="48" customHeight="1" ht="20">
+      <c r="A48" s="5" t="n">
+        <v>88</v>
+      </c>
+      <c r="B48" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M48" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N48" s="7" t="n">
+        <v>45319</v>
+      </c>
+      <c r="O48" s="5"/>
+      <c r="P48" s="7"/>
+    </row>
+    <row r="49" customHeight="1" ht="20">
+      <c r="A49" s="5" t="n">
+        <v>89</v>
+      </c>
+      <c r="B49" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M49" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N49" s="7" t="n">
+        <v>45319</v>
+      </c>
+      <c r="O49" s="5"/>
+      <c r="P49" s="7"/>
+    </row>
+    <row r="50" customHeight="1" ht="20">
+      <c r="A50" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="B50" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M50" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N50" s="7" t="n">
+        <v>45321</v>
+      </c>
+      <c r="O50" s="5"/>
+      <c r="P50" s="7"/>
+    </row>
+    <row r="51" customHeight="1" ht="20">
+      <c r="A51" s="5" t="n">
+        <v>102</v>
+      </c>
+      <c r="B51" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M51" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N51" s="7" t="n">
+        <v>45322</v>
+      </c>
+      <c r="O51" s="5"/>
+      <c r="P51" s="7"/>
+    </row>
+    <row r="52" customHeight="1" ht="20">
+      <c r="A52" s="5" t="n">
+        <v>103</v>
+      </c>
+      <c r="B52" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M52" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N52" s="7" t="n">
+        <v>45322</v>
+      </c>
+      <c r="O52" s="5"/>
+      <c r="P52" s="7"/>
+    </row>
+    <row r="53" customHeight="1" ht="20">
+      <c r="A53" s="5" t="n">
+        <v>104</v>
+      </c>
+      <c r="B53" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M53" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N53" s="7" t="n">
+        <v>45322</v>
+      </c>
+      <c r="O53" s="5"/>
+      <c r="P53" s="7"/>
+    </row>
+    <row r="54" customHeight="1" ht="20">
+      <c r="A54" s="5" t="n">
+        <v>105</v>
+      </c>
+      <c r="B54" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M54" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N54" s="7" t="n">
+        <v>45322</v>
+      </c>
+      <c r="O54" s="5"/>
+      <c r="P54" s="7"/>
+    </row>
+    <row r="55" customHeight="1" ht="20">
+      <c r="A55" s="5" t="n">
+        <v>106</v>
+      </c>
+      <c r="B55" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M55" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N55" s="7" t="n">
+        <v>45322</v>
+      </c>
+      <c r="O55" s="5"/>
+      <c r="P55" s="7"/>
+    </row>
+    <row r="56" customHeight="1" ht="20">
+      <c r="A56" s="5" t="n">
+        <v>107</v>
+      </c>
+      <c r="B56" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M56" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N56" s="7" t="n">
+        <v>45322</v>
+      </c>
+      <c r="O56" s="5"/>
+      <c r="P56" s="7"/>
+    </row>
+    <row r="57" customHeight="1" ht="20">
+      <c r="A57" s="5" t="n">
+        <v>108</v>
+      </c>
+      <c r="B57" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M57" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N57" s="7" t="n">
+        <v>45322</v>
+      </c>
+      <c r="O57" s="5"/>
+      <c r="P57" s="7"/>
+    </row>
+    <row r="58" customHeight="1" ht="20">
+      <c r="A58" s="5" t="n">
+        <v>109</v>
+      </c>
+      <c r="B58" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+      <c r="K58" s="5"/>
+      <c r="L58" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M58" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N58" s="7" t="n">
+        <v>45322</v>
+      </c>
+      <c r="O58" s="5"/>
+      <c r="P58" s="7"/>
+    </row>
+    <row r="59" customHeight="1" ht="20">
+      <c r="A59" s="5" t="n">
+        <v>110</v>
+      </c>
+      <c r="B59" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M59" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N59" s="7" t="n">
+        <v>45322</v>
+      </c>
+      <c r="O59" s="5"/>
+      <c r="P59" s="7"/>
+    </row>
+    <row r="60" customHeight="1" ht="20">
+      <c r="A60" s="5" t="n">
+        <v>111</v>
+      </c>
+      <c r="B60" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M60" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N60" s="7" t="n">
+        <v>45322</v>
+      </c>
+      <c r="O60" s="5"/>
+      <c r="P60" s="7"/>
+    </row>
+    <row r="61" customHeight="1" ht="20">
+      <c r="A61" s="5" t="n">
+        <v>112</v>
+      </c>
+      <c r="B61" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M61" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N61" s="7" t="n">
+        <v>45322</v>
+      </c>
+      <c r="O61" s="5"/>
+      <c r="P61" s="7"/>
+    </row>
+    <row r="62" customHeight="1" ht="20">
+      <c r="A62" s="5" t="n">
+        <v>113</v>
+      </c>
+      <c r="B62" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
+      <c r="K62" s="5"/>
+      <c r="L62" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M62" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N62" s="7" t="n">
+        <v>45322</v>
+      </c>
+      <c r="O62" s="5"/>
+      <c r="P62" s="7"/>
+    </row>
+    <row r="63" customHeight="1" ht="20">
+      <c r="A63" s="5" t="n">
+        <v>114</v>
+      </c>
+      <c r="B63" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
+      <c r="K63" s="5"/>
+      <c r="L63" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M63" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N63" s="7" t="n">
+        <v>45322</v>
+      </c>
+      <c r="O63" s="5"/>
+      <c r="P63" s="7"/>
+    </row>
+    <row r="64" customHeight="1" ht="20">
+      <c r="A64" s="5" t="n">
+        <v>73</v>
+      </c>
+      <c r="B64" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
+      <c r="K64" s="5"/>
+      <c r="L64" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M64" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N64" s="7" t="n">
+        <v>45313</v>
+      </c>
+      <c r="O64" s="5"/>
+      <c r="P64" s="7"/>
+    </row>
+    <row r="65" customHeight="1" ht="20">
+      <c r="A65" s="5" t="n">
+        <v>74</v>
+      </c>
+      <c r="B65" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="I65" s="5"/>
+      <c r="J65" s="5"/>
+      <c r="K65" s="5"/>
+      <c r="L65" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M65" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N65" s="7" t="n">
+        <v>45313</v>
+      </c>
+      <c r="O65" s="5"/>
+      <c r="P65" s="7"/>
+    </row>
+    <row r="66" customHeight="1" ht="20">
+      <c r="A66" s="5" t="n">
+        <v>75</v>
+      </c>
+      <c r="B66" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
+      <c r="K66" s="5"/>
+      <c r="L66" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M66" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N66" s="7" t="n">
+        <v>45313</v>
+      </c>
+      <c r="O66" s="5"/>
+      <c r="P66" s="7"/>
+    </row>
+    <row r="67" customHeight="1" ht="20">
+      <c r="A67" s="5" t="n">
+        <v>76</v>
+      </c>
+      <c r="B67" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="I67" s="5"/>
+      <c r="J67" s="5"/>
+      <c r="K67" s="5"/>
+      <c r="L67" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M67" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N67" s="7" t="n">
+        <v>45313</v>
+      </c>
+      <c r="O67" s="5"/>
+      <c r="P67" s="7"/>
+    </row>
+    <row r="68" customHeight="1" ht="20">
+      <c r="A68" s="5" t="n">
+        <v>77</v>
+      </c>
+      <c r="B68" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="I68" s="5"/>
+      <c r="J68" s="5"/>
+      <c r="K68" s="5"/>
+      <c r="L68" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M68" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N68" s="7" t="n">
+        <v>45313</v>
+      </c>
+      <c r="O68" s="5"/>
+      <c r="P68" s="7"/>
+    </row>
+    <row r="69" customHeight="1" ht="20">
+      <c r="A69" s="5" t="n">
+        <v>78</v>
+      </c>
+      <c r="B69" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="I69" s="5"/>
+      <c r="J69" s="5"/>
+      <c r="K69" s="5"/>
+      <c r="L69" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M69" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N69" s="7" t="n">
+        <v>45313</v>
+      </c>
+      <c r="O69" s="5"/>
+      <c r="P69" s="7"/>
+    </row>
+    <row r="70" customHeight="1" ht="20">
+      <c r="A70" s="5" t="n">
+        <v>83</v>
+      </c>
+      <c r="B70" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="5"/>
+      <c r="L70" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M70" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N70" s="7" t="n">
+        <v>45317</v>
+      </c>
+      <c r="O70" s="5"/>
+      <c r="P70" s="7"/>
+    </row>
+    <row r="71" customHeight="1" ht="20">
+      <c r="A71" s="5" t="n">
+        <v>84</v>
+      </c>
+      <c r="B71" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5"/>
+      <c r="K71" s="5"/>
+      <c r="L71" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M71" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N71" s="7" t="n">
+        <v>45319</v>
+      </c>
+      <c r="O71" s="5"/>
+      <c r="P71" s="7" t="n">
+        <v>45321.4720833333</v>
+      </c>
+    </row>
+    <row r="72" customHeight="1" ht="20">
+      <c r="A72" s="5" t="n">
+        <v>97</v>
+      </c>
+      <c r="B72" s="5" t="n">
+        <v>41</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I72" s="5"/>
+      <c r="J72" s="5"/>
+      <c r="K72" s="5"/>
+      <c r="L72" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M72" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N72" s="7" t="n">
+        <v>45321</v>
+      </c>
+      <c r="O72" s="5"/>
+      <c r="P72" s="7" t="n">
+        <v>45323.6678472222</v>
+      </c>
+    </row>
+    <row r="73" customHeight="1" ht="20">
+      <c r="A73" s="5" t="n">
+        <v>98</v>
+      </c>
+      <c r="B73" s="5" t="n">
+        <v>41</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="I73" s="5"/>
+      <c r="J73" s="5"/>
+      <c r="K73" s="5"/>
+      <c r="L73" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M73" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N73" s="7" t="n">
+        <v>45321</v>
+      </c>
+      <c r="O73" s="5"/>
+      <c r="P73" s="7" t="n">
+        <v>45322.6167824074</v>
+      </c>
+    </row>
+    <row r="74" customHeight="1" ht="20">
+      <c r="A74" s="5" t="n">
+        <v>115</v>
+      </c>
+      <c r="B74" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="I74" s="5"/>
+      <c r="J74" s="5"/>
+      <c r="K74" s="5"/>
+      <c r="L74" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M74" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N74" s="7" t="n">
+        <v>45322</v>
+      </c>
+      <c r="O74" s="5"/>
+      <c r="P74" s="7"/>
+    </row>
+    <row r="75" customHeight="1" ht="20">
+      <c r="A75" s="5" t="n">
+        <v>121</v>
+      </c>
+      <c r="B75" s="5" t="n">
+        <v>47</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="I75" s="5"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="5"/>
+      <c r="L75" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M75" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N75" s="7" t="n">
+        <v>45323</v>
+      </c>
+      <c r="O75" s="5"/>
+      <c r="P75" s="7" t="n">
+        <v>45323.239849537</v>
+      </c>
+    </row>
+    <row r="76" customHeight="1" ht="20">
+      <c r="A76" s="5" t="n">
+        <v>82</v>
+      </c>
+      <c r="B76" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I76" s="5"/>
+      <c r="J76" s="5"/>
+      <c r="K76" s="5"/>
+      <c r="L76" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M76" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N76" s="7" t="n">
+        <v>45315</v>
+      </c>
+      <c r="O76" s="5"/>
+      <c r="P76" s="7"/>
+    </row>
+    <row r="77" customHeight="1" ht="20">
+      <c r="A77" s="5" t="n">
+        <v>92</v>
+      </c>
+      <c r="B77" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I77" s="5"/>
+      <c r="J77" s="5"/>
+      <c r="K77" s="5"/>
+      <c r="L77" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M77" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N77" s="7" t="n">
+        <v>45321</v>
+      </c>
+      <c r="O77" s="5"/>
+      <c r="P77" s="7"/>
+    </row>
+    <row r="78" customHeight="1" ht="20">
+      <c r="A78" s="5" t="n">
+        <v>94</v>
+      </c>
+      <c r="B78" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I78" s="5"/>
+      <c r="J78" s="5"/>
+      <c r="K78" s="5"/>
+      <c r="L78" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M78" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N78" s="7" t="n">
+        <v>45321</v>
+      </c>
+      <c r="O78" s="5"/>
+      <c r="P78" s="7"/>
+    </row>
+    <row r="79" customHeight="1" ht="20">
+      <c r="A79" s="5" t="n">
+        <v>96</v>
+      </c>
+      <c r="B79" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="I79" s="5"/>
+      <c r="J79" s="5"/>
+      <c r="K79" s="5"/>
+      <c r="L79" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M79" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N79" s="7" t="n">
+        <v>45321</v>
+      </c>
+      <c r="O79" s="5"/>
+      <c r="P79" s="7"/>
+    </row>
+    <row r="80" customHeight="1" ht="20">
+      <c r="A80" s="5" t="n">
+        <v>122</v>
+      </c>
+      <c r="B80" s="5" t="n">
+        <v>41</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="I80" s="5"/>
+      <c r="J80" s="5"/>
+      <c r="K80" s="5"/>
+      <c r="L80" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M80" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N80" s="7" t="n">
+        <v>45323</v>
+      </c>
+      <c r="O80" s="5"/>
+      <c r="P80" s="7"/>
+    </row>
+    <row r="81" customHeight="1" ht="20">
+      <c r="A81" s="5" t="n">
+        <v>123</v>
+      </c>
+      <c r="B81" s="5" t="n">
+        <v>41</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="I81" s="5"/>
+      <c r="J81" s="5"/>
+      <c r="K81" s="5"/>
+      <c r="L81" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M81" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N81" s="7" t="n">
+        <v>45323</v>
+      </c>
+      <c r="O81" s="5"/>
+      <c r="P81" s="7"/>
+    </row>
+    <row r="82" customHeight="1" ht="20">
+      <c r="A82" s="5" t="n">
+        <v>126</v>
+      </c>
+      <c r="B82" s="5" t="n">
+        <v>47</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I82" s="5"/>
+      <c r="J82" s="5"/>
+      <c r="K82" s="5"/>
+      <c r="L82" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M82" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N82" s="7" t="n">
+        <v>45323</v>
+      </c>
+      <c r="O82" s="5"/>
+      <c r="P82" s="7"/>
+    </row>
+    <row r="83" customHeight="1" ht="20">
+      <c r="A83" s="5" t="n">
+        <v>71</v>
+      </c>
+      <c r="B83" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="I83" s="5"/>
+      <c r="J83" s="5"/>
+      <c r="K83" s="5"/>
+      <c r="L83" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M83" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N83" s="7" t="n">
+        <v>45313</v>
+      </c>
+      <c r="O83" s="5"/>
+      <c r="P83" s="7"/>
+    </row>
+    <row r="84" customHeight="1" ht="20">
+      <c r="A84" s="5" t="n">
+        <v>79</v>
+      </c>
+      <c r="B84" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="I84" s="5"/>
+      <c r="J84" s="5"/>
+      <c r="K84" s="5"/>
+      <c r="L84" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M84" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N84" s="7" t="n">
+        <v>45315</v>
+      </c>
+      <c r="O84" s="5"/>
+      <c r="P84" s="7"/>
+    </row>
+    <row r="85" customHeight="1" ht="20">
+      <c r="A85" s="5" t="n">
+        <v>80</v>
+      </c>
+      <c r="B85" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="I85" s="5"/>
+      <c r="J85" s="5"/>
+      <c r="K85" s="5"/>
+      <c r="L85" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M85" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N85" s="7" t="n">
+        <v>45315</v>
+      </c>
+      <c r="O85" s="5"/>
+      <c r="P85" s="7"/>
+    </row>
+    <row r="86" customHeight="1" ht="20">
+      <c r="A86" s="5" t="n">
+        <v>81</v>
+      </c>
+      <c r="B86" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="I86" s="5"/>
+      <c r="J86" s="5"/>
+      <c r="K86" s="5"/>
+      <c r="L86" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M86" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N86" s="7" t="n">
+        <v>45315</v>
+      </c>
+      <c r="O86" s="5"/>
+      <c r="P86" s="7" t="n">
+        <v>45315.7295601852</v>
+      </c>
+    </row>
+    <row r="87" customHeight="1" ht="20">
+      <c r="A87" s="5" t="n">
+        <v>91</v>
+      </c>
+      <c r="B87" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="5"/>
+      <c r="J87" s="5"/>
+      <c r="K87" s="5"/>
+      <c r="L87" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M87" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N87" s="7" t="n">
+        <v>45319</v>
+      </c>
+      <c r="O87" s="5"/>
+      <c r="P87" s="7"/>
+    </row>
+    <row r="88" customHeight="1" ht="20">
+      <c r="A88" s="5" t="n">
+        <v>93</v>
+      </c>
+      <c r="B88" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F88" s="6"/>
+      <c r="G88" s="6"/>
+      <c r="H88" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="I88" s="5"/>
+      <c r="J88" s="5"/>
+      <c r="K88" s="5"/>
+      <c r="L88" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M88" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N88" s="7" t="n">
+        <v>45321</v>
+      </c>
+      <c r="O88" s="5"/>
+      <c r="P88" s="7"/>
+    </row>
+    <row r="89" customHeight="1" ht="20">
+      <c r="A89" s="5" t="n">
+        <v>101</v>
+      </c>
+      <c r="B89" s="5" t="n">
+        <v>41</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E89" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I89" s="5"/>
+      <c r="J89" s="5"/>
+      <c r="K89" s="5"/>
+      <c r="L89" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M89" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N89" s="7" t="n">
+        <v>45321</v>
+      </c>
+      <c r="O89" s="5"/>
+      <c r="P89" s="7"/>
+    </row>
+    <row r="90" customHeight="1" ht="20">
+      <c r="A90" s="5" t="n">
+        <v>120</v>
+      </c>
+      <c r="B90" s="5" t="n">
+        <v>46</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E90" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="I90" s="5"/>
+      <c r="J90" s="5"/>
+      <c r="K90" s="5"/>
+      <c r="L90" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M90" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N90" s="7" t="n">
+        <v>45323</v>
+      </c>
+      <c r="O90" s="5"/>
+      <c r="P90" s="7"/>
     </row>
   </sheetData>
   <tableParts count="1">

</xml_diff>